<commit_message>
Calendario, jornadas y clasificacion inicial
</commit_message>
<xml_diff>
--- a/2026/data/jornada_1_inicial.xlsx
+++ b/2026/data/jornada_1_inicial.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_L</t>
+          <t>RTDO L</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -451,17 +451,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_VISITANTE</t>
+          <t>RTDO V</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>jornada</t>
+          <t>Jornada</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_L.1</t>
+          <t>RTDO L.1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_V.1</t>
+          <t>RTDO V.1</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Coquina</t>
+          <t>Gonzo</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -546,12 +546,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Ruso</t>
+          <t>Coquina</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Gonzo</t>
+          <t>Puche</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -585,12 +585,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Ruso</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>Lope</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Puche</t>
         </is>
       </c>
       <c r="I4" t="n">

</xml_diff>